<commit_message>
Se califico el contexto del proyecto
</commit_message>
<xml_diff>
--- a/Project/Context/Context.Score.xlsx
+++ b/Project/Context/Context.Score.xlsx
@@ -1,150 +1,176 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28803"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Dropbox\Tmp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A1DB40-89F2-4833-9F77-1F7E05C9AA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF55138A-9504-4D86-8D69-0DC3A94C8057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43D718D0-2724-4196-A35D-E65845C004B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+  <si>
+    <t>Categorias</t>
+  </si>
+  <si>
+    <t>Especificación</t>
+  </si>
+  <si>
+    <t>Detalle</t>
+  </si>
+  <si>
+    <t>Calificación</t>
+  </si>
+  <si>
+    <t>Observacion</t>
+  </si>
   <si>
     <t>Contexto</t>
   </si>
   <si>
+    <t>Claridad</t>
+  </si>
+  <si>
+    <t>El texto es claro y conciso</t>
+  </si>
+  <si>
+    <t>Completitud</t>
+  </si>
+  <si>
+    <t>El texto es detallado y su idea es consistente</t>
+  </si>
+  <si>
+    <t>Coherencia</t>
+  </si>
+  <si>
+    <t>El texto es coherente con el Diagrama Presentado</t>
+  </si>
+  <si>
+    <t>No hay Diagrama</t>
+  </si>
+  <si>
+    <t>Formato</t>
+  </si>
+  <si>
+    <t>El texto es limpio y sin errores de ortografa o formato</t>
+  </si>
+  <si>
     <t>Requerimientos Funcionales</t>
   </si>
   <si>
+    <t>La descripcion es clara y concisa (una sola idea)</t>
+  </si>
+  <si>
+    <t>Comprensible</t>
+  </si>
+  <si>
+    <t>El detalle es entendible y consistente</t>
+  </si>
+  <si>
+    <t>Coherente</t>
+  </si>
+  <si>
+    <t>El Requerimiento es coherente con los escenarios</t>
+  </si>
+  <si>
+    <t>Completo</t>
+  </si>
+  <si>
+    <t>Incluye al menos un interesado por Requerimiento</t>
+  </si>
+  <si>
     <t>Requerimiento NO Funcionales</t>
   </si>
   <si>
+    <t>El texto es entendible y consistente</t>
+  </si>
+  <si>
+    <t>El texto menciona su metrica y se listan los interesados</t>
+  </si>
+  <si>
     <t>Atributos de Calidad</t>
   </si>
   <si>
+    <t>Cada interesado tiene al menos un atributo calificado</t>
+  </si>
+  <si>
+    <t>Consistente</t>
+  </si>
+  <si>
+    <t>Los valores son consistentes y su suma es 100%</t>
+  </si>
+  <si>
+    <t>Calculos</t>
+  </si>
+  <si>
+    <t>Los calculos de promedio son correctos y ajustados</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>El total de promedios es ajustado y sy suma es el 100%</t>
+  </si>
+  <si>
     <t>Ponderacion</t>
   </si>
   <si>
-    <t>Categorias</t>
-  </si>
-  <si>
-    <t>Completitud</t>
-  </si>
-  <si>
-    <t>Coherencia</t>
-  </si>
-  <si>
-    <t>Claridad</t>
-  </si>
-  <si>
-    <t>Formato</t>
-  </si>
-  <si>
-    <t>El texto es detallado y su idea es consistente</t>
-  </si>
-  <si>
-    <t>El texto es limpio y sin errores de ortografa o formato</t>
-  </si>
-  <si>
-    <t>Especificación</t>
-  </si>
-  <si>
-    <t>Detalle</t>
-  </si>
-  <si>
-    <t>Calificación</t>
-  </si>
-  <si>
-    <t>El texto es claro y conciso</t>
-  </si>
-  <si>
-    <t>Completo</t>
-  </si>
-  <si>
-    <t>Comprensible</t>
-  </si>
-  <si>
-    <t>Coherente</t>
-  </si>
-  <si>
-    <t>La descripcion es clara y concisa (una sola idea)</t>
-  </si>
-  <si>
-    <t>El detalle es entendible y consistente</t>
-  </si>
-  <si>
-    <t>Incluye al menos un interesado por Requerimiento</t>
-  </si>
-  <si>
-    <t>El texto es coherente con el Diagrama Presentado</t>
-  </si>
-  <si>
-    <t>El texto es entendible y consistente</t>
-  </si>
-  <si>
-    <t>El texto menciona su metrica y se listan los interesados</t>
-  </si>
-  <si>
-    <t>El Requerimiento es coherente con los escenarios</t>
-  </si>
-  <si>
-    <t>Cada interesado tiene al menos un atributo calificado</t>
-  </si>
-  <si>
-    <t>Consistente</t>
-  </si>
-  <si>
-    <t>Los valores son consistentes y su suma es 100%</t>
-  </si>
-  <si>
-    <t>Calculos</t>
-  </si>
-  <si>
-    <t>Los calculos de promedio son correctos y ajustados</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>El total de promedios es ajustado y sy suma es el 100%</t>
-  </si>
-  <si>
     <t>Se detalla la categoria y subcategoria</t>
   </si>
   <si>
+    <t>No hay Categoria ni subcategoria</t>
+  </si>
+  <si>
     <t>Clasificacion</t>
   </si>
   <si>
     <t>Se califican los grados de impacto y Dificultad por aca atributo</t>
   </si>
   <si>
+    <t>El calculo se ajusta a: (Impacto + Dificultad) * ponderacion</t>
+  </si>
+  <si>
     <t>Prioridad</t>
   </si>
   <si>
     <t>el Resultado Final Muestra el Orden de mayor a menor</t>
   </si>
   <si>
-    <t>El calculo se ajusta a: (Impacto + Dificultad) * ponderacion</t>
-  </si>
-  <si>
-    <t>Observacion</t>
+    <t>En la prioridad se escapo colocar primero la mantenibilidad, creo yo que es un error que no debe ser tan penalizado por eso le di 0,15</t>
+  </si>
+  <si>
+    <t>Observaciones Finales</t>
+  </si>
+  <si>
+    <t>La presentacion es muy clara y presenta un proyecto muy interesante. Cumple con casi todos los puntos que se deben evaluar a la perfeccion, solo falto el diagrama y colocar las categorias y subcategorias. En la prioridad se escapo colocar primero la mantenibilidad, creo que fue un error que se escapo, se recomienda cambiarlo para que las prioridades queden bien.</t>
   </si>
 </sst>
 </file>
@@ -153,9 +179,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,6 +203,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -205,7 +237,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -314,28 +346,76 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,16 +425,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -667,315 +748,330 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DCA2EC-DA8C-4840-866D-0B6F8056BF9D}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="36.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" thickBot="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="9"/>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="9"/>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="D5" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="12">
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="6">
         <v>0.25</v>
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
+    <row r="7" spans="1:5">
+      <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="2"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="12"/>
+      <c r="B8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="12">
+      <c r="D8" s="6">
         <v>0.25</v>
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="1:5" ht="15" thickBot="1">
+      <c r="A9" s="13"/>
+      <c r="B9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="12">
+      <c r="D10" s="6">
         <v>0.25</v>
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
+    <row r="11" spans="1:5">
+      <c r="A11" s="9"/>
       <c r="B11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="12">
+        <v>24</v>
+      </c>
+      <c r="D11" s="6">
         <v>0.25</v>
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
+    <row r="12" spans="1:5">
+      <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1">
+      <c r="A13" s="10"/>
+      <c r="B13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="12">
+      <c r="D13" s="6">
         <v>0.25</v>
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="4" t="s">
+    <row r="14" spans="1:5">
+      <c r="A14" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="12">
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="6">
         <v>0.25</v>
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
+    <row r="15" spans="1:5">
+      <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="12">
+        <v>29</v>
+      </c>
+      <c r="D15" s="6">
         <v>0.25</v>
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
+    <row r="16" spans="1:5">
+      <c r="A16" s="12"/>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" thickBot="1">
+      <c r="A17" s="13"/>
+      <c r="B17" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E17" s="2"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="6">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="9"/>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="2"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="9"/>
+      <c r="B20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="7" t="s">
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="17"/>
+    </row>
+    <row r="21" spans="1:6" ht="45.75">
+      <c r="A21" s="10"/>
+      <c r="B21" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="16">
+        <v>0.15</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="C22" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="13">
+      <c r="D22" s="7">
         <f>SUM(D2:D21)</f>
-        <v>5</v>
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="152.25">
+      <c r="E24" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update  Context.Score.xlsx with the score
</commit_message>
<xml_diff>
--- a/Project/Context/Context.Score.xlsx
+++ b/Project/Context/Context.Score.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Dropbox\Personal\Cursos\SoftwareArchitecture\Repository\Project\Context\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lilianestefaniamaradiagocorrea/Downloads/SoftwareArchitecture-2025-01-lilmarcor 2/Project/Context/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3BBE2C-8253-4B3C-AD2D-44BC5ACEEBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9088B9-665D-D549-90C6-AEA9798AF270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4164" windowWidth="23256" windowHeight="12456" xr2:uid="{43D718D0-2724-4196-A35D-E65845C004B2}"/>
+    <workbookView xWindow="14800" yWindow="900" windowWidth="14440" windowHeight="16600" xr2:uid="{43D718D0-2724-4196-A35D-E65845C004B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Contexto</t>
   </si>
@@ -123,12 +134,18 @@
     <t>Total</t>
   </si>
   <si>
+    <t>El total de promedios es ajustado y sy suma es el 100%</t>
+  </si>
+  <si>
     <t>Se detalla la categoria y subcategoria</t>
   </si>
   <si>
     <t>Clasificacion</t>
   </si>
   <si>
+    <t>Se califican los grados de impacto y Dificultad por aca atributo</t>
+  </si>
+  <si>
     <t>Prioridad</t>
   </si>
   <si>
@@ -141,10 +158,19 @@
     <t>Observacion</t>
   </si>
   <si>
-    <t>El total de promedios es ajustado y su suma es el 100%</t>
-  </si>
-  <si>
-    <t>Se califican los grados de impacto y Dificultad por dada atributo</t>
+    <t>yo agregaria algo que explique brevemente bajo que criterios hace la seleccion o que es lo que me arroja el analisis: por ejemplo …. Realiza un analisis teniendo en cuenta el modelo de negocio o las necesidades del negocio para el cual esta pensado el espacio. (ese seria el criterio de clasificacion de propiedades)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">me gusta porque tambien incluye criterios de aceptacion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">hace falta la categoria </t>
+  </si>
+  <si>
+    <t>creo que  la multiplicacion del peso se esta haciendo en formato incorrecto, deberia ser 28%, 28/100 o 0.28</t>
+  </si>
+  <si>
+    <t>evaluacion de lilmarcor a dilaspsan</t>
   </si>
 </sst>
 </file>
@@ -152,8 +178,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -179,7 +205,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -204,6 +230,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -317,9 +349,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -330,8 +362,8 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -352,9 +384,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -371,9 +404,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -411,7 +444,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -517,7 +550,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -659,7 +692,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -670,19 +703,19 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -696,10 +729,10 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -714,7 +747,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
@@ -723,11 +756,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -740,7 +775,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10"/>
       <c r="B5" s="4" t="s">
         <v>9</v>
@@ -753,7 +788,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>1</v>
       </c>
@@ -766,9 +801,11 @@
       <c r="D6" s="6">
         <v>0.25</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E6" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="2" t="s">
         <v>17</v>
@@ -781,7 +818,7 @@
       </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="2" t="s">
         <v>18</v>
@@ -794,7 +831,7 @@
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="4" t="s">
         <v>16</v>
@@ -807,7 +844,7 @@
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>2</v>
       </c>
@@ -822,7 +859,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="2" t="s">
         <v>17</v>
@@ -835,7 +872,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="2" t="s">
         <v>18</v>
@@ -848,7 +885,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="4" t="s">
         <v>16</v>
@@ -861,7 +898,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>3</v>
       </c>
@@ -876,7 +913,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="2" t="s">
         <v>27</v>
@@ -889,7 +926,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="2" t="s">
         <v>29</v>
@@ -902,20 +939,20 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
       <c r="B17" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D17" s="6">
         <v>0.25</v>
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
         <v>4</v>
       </c>
@@ -923,59 +960,66 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D18" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19" s="6">
         <v>0.25</v>
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20" s="6">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.18</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D21" s="6">
         <v>0.25</v>
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C22" s="5" t="s">
         <v>31</v>
       </c>
       <c r="D22" s="7">
         <f>SUM(D2:D21)</f>
-        <v>5</v>
+        <v>4.8599999999999994</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add rubric-based evaluation to weighting table
</commit_message>
<xml_diff>
--- a/Project/Context/Context.Score.xlsx
+++ b/Project/Context/Context.Score.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Dropbox\Tmp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jddia\OneDrive\U\SoftwareArchitecture\Project\Context\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A1DB40-89F2-4833-9F77-1F7E05C9AA76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C416714-D1D1-4D0E-9C51-B2B51B35BA44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43D718D0-2724-4196-A35D-E65845C004B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43D718D0-2724-4196-A35D-E65845C004B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>Contexto</t>
   </si>
@@ -60,9 +71,6 @@
     <t>El texto es detallado y su idea es consistente</t>
   </si>
   <si>
-    <t>El texto es limpio y sin errores de ortografa o formato</t>
-  </si>
-  <si>
     <t>Especificación</t>
   </si>
   <si>
@@ -145,6 +153,60 @@
   </si>
   <si>
     <t>Observacion</t>
+  </si>
+  <si>
+    <t>Pequeño error ortográfico en la palabra “proposito”; falta tilde.</t>
+  </si>
+  <si>
+    <t>El texto es limpio y sin errores de ortografía o formato</t>
+  </si>
+  <si>
+    <t>Cada requerimiento presenta una única idea clara.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	El texto es fácil de entender y está redactado con consistencia.</t>
+  </si>
+  <si>
+    <t>Todos los RNF tienen sentido.</t>
+  </si>
+  <si>
+    <t>Todos los requerimientos incluyen una métrica y una lista de interesados.</t>
+  </si>
+  <si>
+    <t>El detalle de cada requerimiento se entiende sin ambigüedades.</t>
+  </si>
+  <si>
+    <t>Cada requerimiento tiene una descripción clara y enfocada en una sola funcionalidad.</t>
+  </si>
+  <si>
+    <t>Cada requerimiento menciona al menos un interesado relevante.</t>
+  </si>
+  <si>
+    <t>Todos los requerimientos están alineados con el sistema descrito.</t>
+  </si>
+  <si>
+    <t>El texto comunica claramente el propósito del proyecto.</t>
+  </si>
+  <si>
+    <t>La información es completa.</t>
+  </si>
+  <si>
+    <t>Todos los stakeholders tienen al menos un atributo calificado</t>
+  </si>
+  <si>
+    <t>Las filas individuales suman 100%</t>
+  </si>
+  <si>
+    <t>Los valores de la fila "Total" parecen bien promediados para cada columna</t>
+  </si>
+  <si>
+    <t>La fila final (Total) suma 100%, tal como se espera.</t>
+  </si>
+  <si>
+    <t>Todos los atributos tienen valores numéricos claros para impacto y dificultad.</t>
+  </si>
+  <si>
+    <t>Se verifica que todos los valores calculados siguen la fórmula.</t>
   </si>
 </sst>
 </file>
@@ -152,7 +214,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -205,7 +267,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -314,28 +376,87 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4"/>
+      </left>
+      <right style="thin">
+        <color theme="4"/>
+      </right>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -345,16 +466,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -371,9 +485,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -411,7 +525,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -517,7 +631,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -659,7 +773,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -669,314 +783,349 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04DCA2EC-DA8C-4840-866D-0B6F8056BF9D}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.77734375" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="78.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
+      <c r="D2" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
+      <c r="D3" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E4" s="11"/>
+    </row>
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="13"/>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E4" s="2"/>
-    </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="2" t="s">
+      <c r="D11" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
+      <c r="B12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="2" t="s">
+      <c r="C12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14"/>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="10"/>
-      <c r="B9" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="16"/>
+      <c r="B15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="16"/>
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="10"/>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="D17" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E18" s="2"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="13"/>
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13"/>
+      <c r="B20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14"/>
+      <c r="B21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="5"/>
-      <c r="B20" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D21" s="12">
-        <v>0.25</v>
-      </c>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C22" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="13">
+      <c r="D21" s="7">
+        <v>0</v>
+      </c>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="6">
         <f>SUM(D2:D21)</f>
-        <v>5</v>
-      </c>
+        <v>4.7</v>
+      </c>
+      <c r="E22" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -987,5 +1136,6 @@
     <mergeCell ref="A18:A21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>